<commit_message>
Rename keys, add tests, edit changelog, update spreedsheats
</commit_message>
<xml_diff>
--- a/test/spreadsheets/Voxa Cli Intents Utterances-only-alexa-no-dialog en-US.xlsx
+++ b/test/spreadsheets/Voxa Cli Intents Utterances-only-alexa-no-dialog en-US.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
   <si>
     <t xml:space="preserve">Intent</t>
   </si>
@@ -81,6 +81,12 @@
     <t xml:space="preserve">slotElicitationRequired</t>
   </si>
   <si>
+    <t xml:space="preserve">parameterName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parameterValue</t>
+  </si>
+  <si>
     <t xml:space="preserve">AMAZON.NextIntent</t>
   </si>
   <si>
@@ -130,6 +136,15 @@
   </si>
   <si>
     <t xml:space="preserve">LIST_OF_BEARS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUMANINTENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fallback skill</t>
   </si>
   <si>
     <t xml:space="preserve">JokeIntent</t>
@@ -231,7 +246,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;BOOL&quot;e&quot;AN&quot;"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -635,36 +650,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R7" activeCellId="0" sqref="O5:R7"/>
+      <selection pane="bottomRight" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.328125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="30.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="26.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="19" style="0" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.42"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,49 +734,55 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="H5" s="4"/>
       <c r="P5" s="4"/>
@@ -773,10 +791,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H6" s="4"/>
       <c r="Q6" s="4"/>
@@ -784,10 +802,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="4"/>
       <c r="Q7" s="4"/>
@@ -795,16 +813,27 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -828,100 +857,100 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D11" activeCellId="1" sqref="O5:R7 D11"/>
+      <selection pane="bottomLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.30078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="24.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="65.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="6" style="3" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="3" width="9.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="6" style="3" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="3" width="9.42"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D7" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D8" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D9" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D10" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D11" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -945,33 +974,32 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="1" sqref="O5:R7 A6"/>
+      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.83"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -995,24 +1023,24 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="O5:R7 A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.30078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="42.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="2" style="3" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="3" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="42.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="2" style="3" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="3" width="9.42"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1036,38 +1064,38 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="O5:R7 A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.30078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="2" style="3" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="3" width="9.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="2" style="3" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="3" width="9.42"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1091,19 +1119,19 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="E21" activeCellId="1" sqref="O5:R7 E21"/>
+      <selection pane="bottomLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.30078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="2" style="3" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="3" width="9.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="2" style="3" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="3" width="9.42"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>4</v>
@@ -1111,18 +1139,18 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>